<commit_message>
Add test: Server sends self-signed certificate, client trusts expired self-signed certificate -> OK
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferstl\git\jdk-tls-experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080229BA-167B-47DB-9031-954253B62EEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FEADBC-0880-45BA-850F-3B98ACDADD66}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30585" yWindow="3630" windowWidth="26265" windowHeight="14955" xr2:uid="{505F494E-320A-4747-AE0A-B62F5B060A82}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="13">
   <si>
     <t>Root CA</t>
   </si>
@@ -136,7 +136,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -148,20 +148,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -475,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6A52E-CEDE-4D7A-9DB5-809A69ADD6EC}">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,13 +733,24 @@
         <v>8</v>
       </c>
     </row>
+    <row r="17" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="I1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:H40">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",A3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>